<commit_message>
implement multi selection for informations page and home page show total informations
</commit_message>
<xml_diff>
--- a/Files/Total/xlsx Files/all_stocks.xlsx
+++ b/Files/Total/xlsx Files/all_stocks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Stock</t>
   </si>
@@ -52,13 +52,28 @@
     <t>-</t>
   </si>
   <si>
-    <t>173.67%</t>
-  </si>
-  <si>
-    <t>-4.45%</t>
-  </si>
-  <si>
-    <t>46.06%</t>
+    <t>34</t>
+  </si>
+  <si>
+    <t>-3</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>34.0</t>
+  </si>
+  <si>
+    <t>253.0%</t>
+  </si>
+  <si>
+    <t>-5.1%</t>
+  </si>
+  <si>
+    <t>40.94%</t>
   </si>
   <si>
     <t>5.12%</t>
@@ -455,78 +470,78 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
-        <v>34</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
       </c>
       <c r="D2">
         <v>102</v>
       </c>
       <c r="E2">
-        <v>8.210000000000001</v>
+        <v>10.59</v>
       </c>
       <c r="F2">
-        <v>279.14</v>
+        <v>360.06</v>
       </c>
       <c r="G2">
-        <v>177.14</v>
+        <v>258.06</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3">
-        <v>34</v>
-      </c>
-      <c r="C3">
-        <v>40</v>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
       </c>
       <c r="D3">
         <v>1360</v>
       </c>
       <c r="E3">
-        <v>38.22</v>
+        <v>37.96</v>
       </c>
       <c r="F3">
-        <v>1299.48</v>
+        <v>1290.64</v>
       </c>
       <c r="G3">
-        <v>-60.52</v>
+        <v>-69.36</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4">
-        <v>-3</v>
-      </c>
-      <c r="C4">
-        <v>34</v>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
       </c>
       <c r="D4">
         <v>-102</v>
       </c>
       <c r="E4">
-        <v>49.66</v>
+        <v>47.92</v>
       </c>
       <c r="F4">
-        <v>-148.98</v>
+        <v>-143.76</v>
       </c>
       <c r="G4">
-        <v>-46.98</v>
+        <v>-41.76</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -552,7 +567,7 @@
         <v>69.63999999999999</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>